<commit_message>
Add overall sheet to QA documentation
Co-Authored-By: Stoyan Skuliev <106760018+SGSkuliev21@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/Baklava_-_QA_Documentation.xlsx
+++ b/docs/Baklava_-_QA_Documentation.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivelin\Documents\baklava\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4925A0-C1B7-4E31-BBEB-CC8B21303CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4DD221-BAD1-4A8F-9CF9-BA0FFC7BAB48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{15209598-3E61-4671-B5D6-5F4A7C929687}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{15209598-3E61-4671-B5D6-5F4A7C929687}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Menu" sheetId="1" r:id="rId1"/>
-    <sheet name="Lose Screen" sheetId="2" r:id="rId2"/>
-    <sheet name="Victory Screen" sheetId="3" r:id="rId3"/>
+    <sheet name="Gameplay" sheetId="4" r:id="rId2"/>
+    <sheet name="Lose Screen" sheetId="2" r:id="rId3"/>
+    <sheet name="Victory Screen" sheetId="3" r:id="rId4"/>
+    <sheet name="Overall " sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="75">
   <si>
     <t>Test Case 1</t>
   </si>
@@ -111,6 +113,9 @@
     <t>Test Case 13</t>
   </si>
   <si>
+    <t>Test Case 14</t>
+  </si>
+  <si>
     <t>Ivelin Bozhilov</t>
   </si>
   <si>
@@ -190,6 +195,75 @@
   </si>
   <si>
     <t>Result check</t>
+  </si>
+  <si>
+    <t>Baklava TD - QA Dovumentation | Overall</t>
+  </si>
+  <si>
+    <t>Overall check</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>0 | 0.0%</t>
+  </si>
+  <si>
+    <t>Not tested</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0 | 0.0%</t>
+  </si>
+  <si>
+    <t>Total Tests</t>
+  </si>
+  <si>
+    <t>Total score</t>
+  </si>
+  <si>
+    <t>Baklava TD - QA Dovumentation | Gameplay</t>
+  </si>
+  <si>
+    <t>Gameplay</t>
+  </si>
+  <si>
+    <t>Test Case 4</t>
+  </si>
+  <si>
+    <t>Test Case 9</t>
+  </si>
+  <si>
+    <t>Test Case 5</t>
+  </si>
+  <si>
+    <t>Test Case 15</t>
+  </si>
+  <si>
+    <t>Test Case 16</t>
+  </si>
+  <si>
+    <t>Test Case 17</t>
+  </si>
+  <si>
+    <t>Test Case 18</t>
+  </si>
+  <si>
+    <t>Test Case 19</t>
+  </si>
+  <si>
+    <t>Test Case 20</t>
+  </si>
+  <si>
+    <t>20 | 100.0%</t>
   </si>
 </sst>
 </file>
@@ -329,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -369,6 +443,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -686,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A3805D7-8844-4E6B-BC59-814E106A8F59}">
   <dimension ref="C1:O56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:O20"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="J78" sqref="J78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -815,7 +892,7 @@
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
@@ -825,7 +902,7 @@
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
@@ -853,7 +930,7 @@
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
@@ -918,21 +995,21 @@
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>12</v>
@@ -1054,7 +1131,7 @@
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -1064,7 +1141,7 @@
       </c>
       <c r="J28" s="3"/>
       <c r="K28" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
@@ -1092,7 +1169,7 @@
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
@@ -1153,25 +1230,25 @@
     </row>
     <row r="34" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C34" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L34" s="4"/>
       <c r="M34" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N34" s="2" t="s">
         <v>12</v>
@@ -1293,7 +1370,7 @@
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
@@ -1303,7 +1380,7 @@
       </c>
       <c r="J46" s="3"/>
       <c r="K46" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L46" s="5"/>
       <c r="M46" s="5"/>
@@ -1331,7 +1408,7 @@
       </c>
       <c r="D48" s="7"/>
       <c r="E48" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
@@ -1392,25 +1469,25 @@
     </row>
     <row r="52" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C52" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
       <c r="I52" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J52" s="5"/>
       <c r="K52" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="L52" s="4"/>
       <c r="M52" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N52" s="2" t="s">
         <v>12</v>
@@ -1550,22 +1627,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F4FE71-C6FC-40D1-BEB8-75091FEF9EE0}">
-  <dimension ref="C1:O56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E38D76E-95FE-4D0A-B5FB-E607E1A67E56}">
+  <dimension ref="C1:O164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:O20"/>
+      <selection activeCell="C150" sqref="C150:O151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="12" max="12" width="18.88671875" customWidth="1"/>
-    <col min="13" max="13" width="27.5546875" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" customWidth="1"/>
+    <col min="12" max="12" width="21.109375" customWidth="1"/>
+    <col min="13" max="13" width="28.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C1" s="13" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
@@ -1625,9 +1703,2343 @@
       <c r="N4" s="13"/>
       <c r="O4" s="13"/>
     </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C6" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+    </row>
+    <row r="9" spans="3:15" ht="21" x14ac:dyDescent="0.4">
+      <c r="C9" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="K10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C12" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C13" s="8"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+    </row>
+    <row r="15" spans="3:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="C15" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L15" s="3"/>
+      <c r="M15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O16" s="2"/>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C24" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+    </row>
+    <row r="27" spans="3:15" ht="21" x14ac:dyDescent="0.4">
+      <c r="C27" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J28" s="3"/>
+      <c r="K28" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+    </row>
+    <row r="30" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C30" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="7"/>
+      <c r="E30" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J30" s="3"/>
+      <c r="K30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+    </row>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C31" s="8"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+    </row>
+    <row r="33" spans="3:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="C33" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="10"/>
+      <c r="E33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L33" s="3"/>
+      <c r="M33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N33" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O33" s="3"/>
+    </row>
+    <row r="34" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O34" s="2"/>
+    </row>
+    <row r="35" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+    </row>
+    <row r="36" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+    </row>
+    <row r="37" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+    </row>
+    <row r="38" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+    </row>
+    <row r="42" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C42" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="11"/>
+      <c r="K42" s="11"/>
+      <c r="L42" s="11"/>
+      <c r="M42" s="11"/>
+      <c r="N42" s="11"/>
+      <c r="O42" s="11"/>
+    </row>
+    <row r="43" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="11"/>
+      <c r="K43" s="11"/>
+      <c r="L43" s="11"/>
+      <c r="M43" s="11"/>
+      <c r="N43" s="11"/>
+      <c r="O43" s="11"/>
+    </row>
+    <row r="45" spans="3:15" ht="21" x14ac:dyDescent="0.4">
+      <c r="C45" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="12"/>
+      <c r="K45" s="12"/>
+      <c r="L45" s="12"/>
+      <c r="M45" s="12"/>
+      <c r="N45" s="12"/>
+      <c r="O45" s="12"/>
+    </row>
+    <row r="46" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C46" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J46" s="3"/>
+      <c r="K46" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+      <c r="N46" s="5"/>
+      <c r="O46" s="5"/>
+    </row>
+    <row r="47" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5"/>
+      <c r="N47" s="5"/>
+      <c r="O47" s="5"/>
+    </row>
+    <row r="48" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C48" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" s="7"/>
+      <c r="E48" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J48" s="3"/>
+      <c r="K48" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="2"/>
+    </row>
+    <row r="49" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C49" s="8"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="2"/>
+    </row>
+    <row r="51" spans="3:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="C51" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51" s="10"/>
+      <c r="E51" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L51" s="3"/>
+      <c r="M51" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N51" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O51" s="3"/>
+    </row>
+    <row r="52" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C52" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" s="3"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4"/>
+      <c r="L52" s="4"/>
+      <c r="M52" s="4"/>
+      <c r="N52" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O52" s="2"/>
+    </row>
+    <row r="53" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+      <c r="L53" s="4"/>
+      <c r="M53" s="4"/>
+      <c r="N53" s="2"/>
+      <c r="O53" s="2"/>
+    </row>
+    <row r="54" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+      <c r="L54" s="4"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="2"/>
+      <c r="O54" s="2"/>
+    </row>
+    <row r="55" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="4"/>
+      <c r="L55" s="4"/>
+      <c r="M55" s="4"/>
+      <c r="N55" s="2"/>
+      <c r="O55" s="2"/>
+    </row>
+    <row r="56" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="4"/>
+      <c r="L56" s="4"/>
+      <c r="M56" s="4"/>
+      <c r="N56" s="2"/>
+      <c r="O56" s="2"/>
+    </row>
+    <row r="60" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C60" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D60" s="11"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="11"/>
+      <c r="I60" s="11"/>
+      <c r="J60" s="11"/>
+      <c r="K60" s="11"/>
+      <c r="L60" s="11"/>
+      <c r="M60" s="11"/>
+      <c r="N60" s="11"/>
+      <c r="O60" s="11"/>
+    </row>
+    <row r="61" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="11"/>
+      <c r="I61" s="11"/>
+      <c r="J61" s="11"/>
+      <c r="K61" s="11"/>
+      <c r="L61" s="11"/>
+      <c r="M61" s="11"/>
+      <c r="N61" s="11"/>
+      <c r="O61" s="11"/>
+    </row>
+    <row r="63" spans="3:15" ht="21" x14ac:dyDescent="0.4">
+      <c r="C63" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D63" s="12"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="12"/>
+      <c r="G63" s="12"/>
+      <c r="H63" s="12"/>
+      <c r="I63" s="12"/>
+      <c r="J63" s="12"/>
+      <c r="K63" s="12"/>
+      <c r="L63" s="12"/>
+      <c r="M63" s="12"/>
+      <c r="N63" s="12"/>
+      <c r="O63" s="12"/>
+    </row>
+    <row r="64" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C64" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D64" s="3"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J64" s="3"/>
+      <c r="K64" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L64" s="5"/>
+      <c r="M64" s="5"/>
+      <c r="N64" s="5"/>
+      <c r="O64" s="5"/>
+    </row>
+    <row r="65" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5"/>
+      <c r="I65" s="3"/>
+      <c r="J65" s="3"/>
+      <c r="K65" s="5"/>
+      <c r="L65" s="5"/>
+      <c r="M65" s="5"/>
+      <c r="N65" s="5"/>
+      <c r="O65" s="5"/>
+    </row>
+    <row r="66" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C66" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D66" s="7"/>
+      <c r="E66" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J66" s="3"/>
+      <c r="K66" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L66" s="2"/>
+      <c r="M66" s="2"/>
+      <c r="N66" s="2"/>
+      <c r="O66" s="2"/>
+    </row>
+    <row r="67" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C67" s="8"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="2"/>
+      <c r="L67" s="2"/>
+      <c r="M67" s="2"/>
+      <c r="N67" s="2"/>
+      <c r="O67" s="2"/>
+    </row>
+    <row r="69" spans="3:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="C69" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D69" s="10"/>
+      <c r="E69" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+      <c r="I69" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J69" s="3"/>
+      <c r="K69" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L69" s="3"/>
+      <c r="M69" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N69" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O69" s="3"/>
+    </row>
+    <row r="70" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C70" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D70" s="3"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
+      <c r="G70" s="4"/>
+      <c r="H70" s="4"/>
+      <c r="I70" s="4"/>
+      <c r="J70" s="4"/>
+      <c r="K70" s="4"/>
+      <c r="L70" s="4"/>
+      <c r="M70" s="4"/>
+      <c r="N70" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O70" s="2"/>
+    </row>
+    <row r="71" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="4"/>
+      <c r="G71" s="4"/>
+      <c r="H71" s="4"/>
+      <c r="I71" s="4"/>
+      <c r="J71" s="4"/>
+      <c r="K71" s="4"/>
+      <c r="L71" s="4"/>
+      <c r="M71" s="4"/>
+      <c r="N71" s="2"/>
+      <c r="O71" s="2"/>
+    </row>
+    <row r="72" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="4"/>
+      <c r="G72" s="4"/>
+      <c r="H72" s="4"/>
+      <c r="I72" s="4"/>
+      <c r="J72" s="4"/>
+      <c r="K72" s="4"/>
+      <c r="L72" s="4"/>
+      <c r="M72" s="4"/>
+      <c r="N72" s="2"/>
+      <c r="O72" s="2"/>
+    </row>
+    <row r="73" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
+      <c r="G73" s="4"/>
+      <c r="H73" s="4"/>
+      <c r="I73" s="4"/>
+      <c r="J73" s="4"/>
+      <c r="K73" s="4"/>
+      <c r="L73" s="4"/>
+      <c r="M73" s="4"/>
+      <c r="N73" s="2"/>
+      <c r="O73" s="2"/>
+    </row>
+    <row r="74" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="4"/>
+      <c r="F74" s="4"/>
+      <c r="G74" s="4"/>
+      <c r="H74" s="4"/>
+      <c r="I74" s="4"/>
+      <c r="J74" s="4"/>
+      <c r="K74" s="4"/>
+      <c r="L74" s="4"/>
+      <c r="M74" s="4"/>
+      <c r="N74" s="2"/>
+      <c r="O74" s="2"/>
+    </row>
+    <row r="78" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C78" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D78" s="11"/>
+      <c r="E78" s="11"/>
+      <c r="F78" s="11"/>
+      <c r="G78" s="11"/>
+      <c r="H78" s="11"/>
+      <c r="I78" s="11"/>
+      <c r="J78" s="11"/>
+      <c r="K78" s="11"/>
+      <c r="L78" s="11"/>
+      <c r="M78" s="11"/>
+      <c r="N78" s="11"/>
+      <c r="O78" s="11"/>
+    </row>
+    <row r="79" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C79" s="11"/>
+      <c r="D79" s="11"/>
+      <c r="E79" s="11"/>
+      <c r="F79" s="11"/>
+      <c r="G79" s="11"/>
+      <c r="H79" s="11"/>
+      <c r="I79" s="11"/>
+      <c r="J79" s="11"/>
+      <c r="K79" s="11"/>
+      <c r="L79" s="11"/>
+      <c r="M79" s="11"/>
+      <c r="N79" s="11"/>
+      <c r="O79" s="11"/>
+    </row>
+    <row r="81" spans="3:15" ht="21" x14ac:dyDescent="0.4">
+      <c r="C81" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D81" s="12"/>
+      <c r="E81" s="12"/>
+      <c r="F81" s="12"/>
+      <c r="G81" s="12"/>
+      <c r="H81" s="12"/>
+      <c r="I81" s="12"/>
+      <c r="J81" s="12"/>
+      <c r="K81" s="12"/>
+      <c r="L81" s="12"/>
+      <c r="M81" s="12"/>
+      <c r="N81" s="12"/>
+      <c r="O81" s="12"/>
+    </row>
+    <row r="82" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C82" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D82" s="3"/>
+      <c r="E82" s="5"/>
+      <c r="F82" s="5"/>
+      <c r="G82" s="5"/>
+      <c r="H82" s="5"/>
+      <c r="I82" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J82" s="3"/>
+      <c r="K82" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L82" s="5"/>
+      <c r="M82" s="5"/>
+      <c r="N82" s="5"/>
+      <c r="O82" s="5"/>
+    </row>
+    <row r="83" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="5"/>
+      <c r="F83" s="5"/>
+      <c r="G83" s="5"/>
+      <c r="H83" s="5"/>
+      <c r="I83" s="3"/>
+      <c r="J83" s="3"/>
+      <c r="K83" s="5"/>
+      <c r="L83" s="5"/>
+      <c r="M83" s="5"/>
+      <c r="N83" s="5"/>
+      <c r="O83" s="5"/>
+    </row>
+    <row r="84" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C84" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D84" s="7"/>
+      <c r="E84" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F84" s="5"/>
+      <c r="G84" s="5"/>
+      <c r="H84" s="5"/>
+      <c r="I84" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J84" s="3"/>
+      <c r="K84" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L84" s="2"/>
+      <c r="M84" s="2"/>
+      <c r="N84" s="2"/>
+      <c r="O84" s="2"/>
+    </row>
+    <row r="85" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C85" s="8"/>
+      <c r="D85" s="9"/>
+      <c r="E85" s="5"/>
+      <c r="F85" s="5"/>
+      <c r="G85" s="5"/>
+      <c r="H85" s="5"/>
+      <c r="I85" s="3"/>
+      <c r="J85" s="3"/>
+      <c r="K85" s="2"/>
+      <c r="L85" s="2"/>
+      <c r="M85" s="2"/>
+      <c r="N85" s="2"/>
+      <c r="O85" s="2"/>
+    </row>
+    <row r="87" spans="3:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="C87" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D87" s="10"/>
+      <c r="E87" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F87" s="3"/>
+      <c r="G87" s="3"/>
+      <c r="H87" s="3"/>
+      <c r="I87" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J87" s="3"/>
+      <c r="K87" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L87" s="3"/>
+      <c r="M87" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N87" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O87" s="3"/>
+    </row>
+    <row r="88" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C88" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D88" s="3"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="4"/>
+      <c r="G88" s="4"/>
+      <c r="H88" s="4"/>
+      <c r="I88" s="4"/>
+      <c r="J88" s="4"/>
+      <c r="K88" s="4"/>
+      <c r="L88" s="4"/>
+      <c r="M88" s="4"/>
+      <c r="N88" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O88" s="2"/>
+    </row>
+    <row r="89" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="4"/>
+      <c r="G89" s="4"/>
+      <c r="H89" s="4"/>
+      <c r="I89" s="4"/>
+      <c r="J89" s="4"/>
+      <c r="K89" s="4"/>
+      <c r="L89" s="4"/>
+      <c r="M89" s="4"/>
+      <c r="N89" s="2"/>
+      <c r="O89" s="2"/>
+    </row>
+    <row r="90" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="4"/>
+      <c r="G90" s="4"/>
+      <c r="H90" s="4"/>
+      <c r="I90" s="4"/>
+      <c r="J90" s="4"/>
+      <c r="K90" s="4"/>
+      <c r="L90" s="4"/>
+      <c r="M90" s="4"/>
+      <c r="N90" s="2"/>
+      <c r="O90" s="2"/>
+    </row>
+    <row r="91" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="4"/>
+      <c r="F91" s="4"/>
+      <c r="G91" s="4"/>
+      <c r="H91" s="4"/>
+      <c r="I91" s="4"/>
+      <c r="J91" s="4"/>
+      <c r="K91" s="4"/>
+      <c r="L91" s="4"/>
+      <c r="M91" s="4"/>
+      <c r="N91" s="2"/>
+      <c r="O91" s="2"/>
+    </row>
+    <row r="92" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="4"/>
+      <c r="G92" s="4"/>
+      <c r="H92" s="4"/>
+      <c r="I92" s="4"/>
+      <c r="J92" s="4"/>
+      <c r="K92" s="4"/>
+      <c r="L92" s="4"/>
+      <c r="M92" s="4"/>
+      <c r="N92" s="2"/>
+      <c r="O92" s="2"/>
+    </row>
+    <row r="96" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C96" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D96" s="11"/>
+      <c r="E96" s="11"/>
+      <c r="F96" s="11"/>
+      <c r="G96" s="11"/>
+      <c r="H96" s="11"/>
+      <c r="I96" s="11"/>
+      <c r="J96" s="11"/>
+      <c r="K96" s="11"/>
+      <c r="L96" s="11"/>
+      <c r="M96" s="11"/>
+      <c r="N96" s="11"/>
+      <c r="O96" s="11"/>
+    </row>
+    <row r="97" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C97" s="11"/>
+      <c r="D97" s="11"/>
+      <c r="E97" s="11"/>
+      <c r="F97" s="11"/>
+      <c r="G97" s="11"/>
+      <c r="H97" s="11"/>
+      <c r="I97" s="11"/>
+      <c r="J97" s="11"/>
+      <c r="K97" s="11"/>
+      <c r="L97" s="11"/>
+      <c r="M97" s="11"/>
+      <c r="N97" s="11"/>
+      <c r="O97" s="11"/>
+    </row>
+    <row r="99" spans="3:15" ht="21" x14ac:dyDescent="0.4">
+      <c r="C99" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D99" s="12"/>
+      <c r="E99" s="12"/>
+      <c r="F99" s="12"/>
+      <c r="G99" s="12"/>
+      <c r="H99" s="12"/>
+      <c r="I99" s="12"/>
+      <c r="J99" s="12"/>
+      <c r="K99" s="12"/>
+      <c r="L99" s="12"/>
+      <c r="M99" s="12"/>
+      <c r="N99" s="12"/>
+      <c r="O99" s="12"/>
+    </row>
+    <row r="100" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C100" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D100" s="3"/>
+      <c r="E100" s="5"/>
+      <c r="F100" s="5"/>
+      <c r="G100" s="5"/>
+      <c r="H100" s="5"/>
+      <c r="I100" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J100" s="3"/>
+      <c r="K100" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L100" s="5"/>
+      <c r="M100" s="5"/>
+      <c r="N100" s="5"/>
+      <c r="O100" s="5"/>
+    </row>
+    <row r="101" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C101" s="3"/>
+      <c r="D101" s="3"/>
+      <c r="E101" s="5"/>
+      <c r="F101" s="5"/>
+      <c r="G101" s="5"/>
+      <c r="H101" s="5"/>
+      <c r="I101" s="3"/>
+      <c r="J101" s="3"/>
+      <c r="K101" s="5"/>
+      <c r="L101" s="5"/>
+      <c r="M101" s="5"/>
+      <c r="N101" s="5"/>
+      <c r="O101" s="5"/>
+    </row>
+    <row r="102" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C102" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D102" s="7"/>
+      <c r="E102" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F102" s="5"/>
+      <c r="G102" s="5"/>
+      <c r="H102" s="5"/>
+      <c r="I102" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J102" s="3"/>
+      <c r="K102" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L102" s="2"/>
+      <c r="M102" s="2"/>
+      <c r="N102" s="2"/>
+      <c r="O102" s="2"/>
+    </row>
+    <row r="103" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C103" s="8"/>
+      <c r="D103" s="9"/>
+      <c r="E103" s="5"/>
+      <c r="F103" s="5"/>
+      <c r="G103" s="5"/>
+      <c r="H103" s="5"/>
+      <c r="I103" s="3"/>
+      <c r="J103" s="3"/>
+      <c r="K103" s="2"/>
+      <c r="L103" s="2"/>
+      <c r="M103" s="2"/>
+      <c r="N103" s="2"/>
+      <c r="O103" s="2"/>
+    </row>
+    <row r="105" spans="3:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="C105" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D105" s="10"/>
+      <c r="E105" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F105" s="3"/>
+      <c r="G105" s="3"/>
+      <c r="H105" s="3"/>
+      <c r="I105" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J105" s="3"/>
+      <c r="K105" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L105" s="3"/>
+      <c r="M105" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N105" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O105" s="3"/>
+    </row>
+    <row r="106" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C106" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D106" s="3"/>
+      <c r="E106" s="4"/>
+      <c r="F106" s="4"/>
+      <c r="G106" s="4"/>
+      <c r="H106" s="4"/>
+      <c r="I106" s="4"/>
+      <c r="J106" s="4"/>
+      <c r="K106" s="4"/>
+      <c r="L106" s="4"/>
+      <c r="M106" s="4"/>
+      <c r="N106" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O106" s="2"/>
+    </row>
+    <row r="107" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C107" s="3"/>
+      <c r="D107" s="3"/>
+      <c r="E107" s="4"/>
+      <c r="F107" s="4"/>
+      <c r="G107" s="4"/>
+      <c r="H107" s="4"/>
+      <c r="I107" s="4"/>
+      <c r="J107" s="4"/>
+      <c r="K107" s="4"/>
+      <c r="L107" s="4"/>
+      <c r="M107" s="4"/>
+      <c r="N107" s="2"/>
+      <c r="O107" s="2"/>
+    </row>
+    <row r="108" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C108" s="3"/>
+      <c r="D108" s="3"/>
+      <c r="E108" s="4"/>
+      <c r="F108" s="4"/>
+      <c r="G108" s="4"/>
+      <c r="H108" s="4"/>
+      <c r="I108" s="4"/>
+      <c r="J108" s="4"/>
+      <c r="K108" s="4"/>
+      <c r="L108" s="4"/>
+      <c r="M108" s="4"/>
+      <c r="N108" s="2"/>
+      <c r="O108" s="2"/>
+    </row>
+    <row r="109" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C109" s="3"/>
+      <c r="D109" s="3"/>
+      <c r="E109" s="4"/>
+      <c r="F109" s="4"/>
+      <c r="G109" s="4"/>
+      <c r="H109" s="4"/>
+      <c r="I109" s="4"/>
+      <c r="J109" s="4"/>
+      <c r="K109" s="4"/>
+      <c r="L109" s="4"/>
+      <c r="M109" s="4"/>
+      <c r="N109" s="2"/>
+      <c r="O109" s="2"/>
+    </row>
+    <row r="110" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C110" s="3"/>
+      <c r="D110" s="3"/>
+      <c r="E110" s="4"/>
+      <c r="F110" s="4"/>
+      <c r="G110" s="4"/>
+      <c r="H110" s="4"/>
+      <c r="I110" s="4"/>
+      <c r="J110" s="4"/>
+      <c r="K110" s="4"/>
+      <c r="L110" s="4"/>
+      <c r="M110" s="4"/>
+      <c r="N110" s="2"/>
+      <c r="O110" s="2"/>
+    </row>
+    <row r="114" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C114" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D114" s="11"/>
+      <c r="E114" s="11"/>
+      <c r="F114" s="11"/>
+      <c r="G114" s="11"/>
+      <c r="H114" s="11"/>
+      <c r="I114" s="11"/>
+      <c r="J114" s="11"/>
+      <c r="K114" s="11"/>
+      <c r="L114" s="11"/>
+      <c r="M114" s="11"/>
+      <c r="N114" s="11"/>
+      <c r="O114" s="11"/>
+    </row>
+    <row r="115" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C115" s="11"/>
+      <c r="D115" s="11"/>
+      <c r="E115" s="11"/>
+      <c r="F115" s="11"/>
+      <c r="G115" s="11"/>
+      <c r="H115" s="11"/>
+      <c r="I115" s="11"/>
+      <c r="J115" s="11"/>
+      <c r="K115" s="11"/>
+      <c r="L115" s="11"/>
+      <c r="M115" s="11"/>
+      <c r="N115" s="11"/>
+      <c r="O115" s="11"/>
+    </row>
+    <row r="117" spans="3:15" ht="21" x14ac:dyDescent="0.4">
+      <c r="C117" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D117" s="12"/>
+      <c r="E117" s="12"/>
+      <c r="F117" s="12"/>
+      <c r="G117" s="12"/>
+      <c r="H117" s="12"/>
+      <c r="I117" s="12"/>
+      <c r="J117" s="12"/>
+      <c r="K117" s="12"/>
+      <c r="L117" s="12"/>
+      <c r="M117" s="12"/>
+      <c r="N117" s="12"/>
+      <c r="O117" s="12"/>
+    </row>
+    <row r="118" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C118" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D118" s="3"/>
+      <c r="E118" s="5"/>
+      <c r="F118" s="5"/>
+      <c r="G118" s="5"/>
+      <c r="H118" s="5"/>
+      <c r="I118" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J118" s="3"/>
+      <c r="K118" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L118" s="5"/>
+      <c r="M118" s="5"/>
+      <c r="N118" s="5"/>
+      <c r="O118" s="5"/>
+    </row>
+    <row r="119" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C119" s="3"/>
+      <c r="D119" s="3"/>
+      <c r="E119" s="5"/>
+      <c r="F119" s="5"/>
+      <c r="G119" s="5"/>
+      <c r="H119" s="5"/>
+      <c r="I119" s="3"/>
+      <c r="J119" s="3"/>
+      <c r="K119" s="5"/>
+      <c r="L119" s="5"/>
+      <c r="M119" s="5"/>
+      <c r="N119" s="5"/>
+      <c r="O119" s="5"/>
+    </row>
+    <row r="120" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C120" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D120" s="7"/>
+      <c r="E120" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F120" s="5"/>
+      <c r="G120" s="5"/>
+      <c r="H120" s="5"/>
+      <c r="I120" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J120" s="3"/>
+      <c r="K120" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L120" s="2"/>
+      <c r="M120" s="2"/>
+      <c r="N120" s="2"/>
+      <c r="O120" s="2"/>
+    </row>
+    <row r="121" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C121" s="8"/>
+      <c r="D121" s="9"/>
+      <c r="E121" s="5"/>
+      <c r="F121" s="5"/>
+      <c r="G121" s="5"/>
+      <c r="H121" s="5"/>
+      <c r="I121" s="3"/>
+      <c r="J121" s="3"/>
+      <c r="K121" s="2"/>
+      <c r="L121" s="2"/>
+      <c r="M121" s="2"/>
+      <c r="N121" s="2"/>
+      <c r="O121" s="2"/>
+    </row>
+    <row r="123" spans="3:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="C123" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D123" s="10"/>
+      <c r="E123" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F123" s="3"/>
+      <c r="G123" s="3"/>
+      <c r="H123" s="3"/>
+      <c r="I123" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J123" s="3"/>
+      <c r="K123" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L123" s="3"/>
+      <c r="M123" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N123" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O123" s="3"/>
+    </row>
+    <row r="124" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C124" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D124" s="3"/>
+      <c r="E124" s="4"/>
+      <c r="F124" s="4"/>
+      <c r="G124" s="4"/>
+      <c r="H124" s="4"/>
+      <c r="I124" s="4"/>
+      <c r="J124" s="4"/>
+      <c r="K124" s="4"/>
+      <c r="L124" s="4"/>
+      <c r="M124" s="4"/>
+      <c r="N124" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O124" s="2"/>
+    </row>
+    <row r="125" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C125" s="3"/>
+      <c r="D125" s="3"/>
+      <c r="E125" s="4"/>
+      <c r="F125" s="4"/>
+      <c r="G125" s="4"/>
+      <c r="H125" s="4"/>
+      <c r="I125" s="4"/>
+      <c r="J125" s="4"/>
+      <c r="K125" s="4"/>
+      <c r="L125" s="4"/>
+      <c r="M125" s="4"/>
+      <c r="N125" s="2"/>
+      <c r="O125" s="2"/>
+    </row>
+    <row r="126" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C126" s="3"/>
+      <c r="D126" s="3"/>
+      <c r="E126" s="4"/>
+      <c r="F126" s="4"/>
+      <c r="G126" s="4"/>
+      <c r="H126" s="4"/>
+      <c r="I126" s="4"/>
+      <c r="J126" s="4"/>
+      <c r="K126" s="4"/>
+      <c r="L126" s="4"/>
+      <c r="M126" s="4"/>
+      <c r="N126" s="2"/>
+      <c r="O126" s="2"/>
+    </row>
+    <row r="127" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C127" s="3"/>
+      <c r="D127" s="3"/>
+      <c r="E127" s="4"/>
+      <c r="F127" s="4"/>
+      <c r="G127" s="4"/>
+      <c r="H127" s="4"/>
+      <c r="I127" s="4"/>
+      <c r="J127" s="4"/>
+      <c r="K127" s="4"/>
+      <c r="L127" s="4"/>
+      <c r="M127" s="4"/>
+      <c r="N127" s="2"/>
+      <c r="O127" s="2"/>
+    </row>
+    <row r="128" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C128" s="3"/>
+      <c r="D128" s="3"/>
+      <c r="E128" s="4"/>
+      <c r="F128" s="4"/>
+      <c r="G128" s="4"/>
+      <c r="H128" s="4"/>
+      <c r="I128" s="4"/>
+      <c r="J128" s="4"/>
+      <c r="K128" s="4"/>
+      <c r="L128" s="4"/>
+      <c r="M128" s="4"/>
+      <c r="N128" s="2"/>
+      <c r="O128" s="2"/>
+    </row>
+    <row r="132" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C132" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D132" s="11"/>
+      <c r="E132" s="11"/>
+      <c r="F132" s="11"/>
+      <c r="G132" s="11"/>
+      <c r="H132" s="11"/>
+      <c r="I132" s="11"/>
+      <c r="J132" s="11"/>
+      <c r="K132" s="11"/>
+      <c r="L132" s="11"/>
+      <c r="M132" s="11"/>
+      <c r="N132" s="11"/>
+      <c r="O132" s="11"/>
+    </row>
+    <row r="133" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C133" s="11"/>
+      <c r="D133" s="11"/>
+      <c r="E133" s="11"/>
+      <c r="F133" s="11"/>
+      <c r="G133" s="11"/>
+      <c r="H133" s="11"/>
+      <c r="I133" s="11"/>
+      <c r="J133" s="11"/>
+      <c r="K133" s="11"/>
+      <c r="L133" s="11"/>
+      <c r="M133" s="11"/>
+      <c r="N133" s="11"/>
+      <c r="O133" s="11"/>
+    </row>
+    <row r="135" spans="3:15" ht="21" x14ac:dyDescent="0.4">
+      <c r="C135" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D135" s="12"/>
+      <c r="E135" s="12"/>
+      <c r="F135" s="12"/>
+      <c r="G135" s="12"/>
+      <c r="H135" s="12"/>
+      <c r="I135" s="12"/>
+      <c r="J135" s="12"/>
+      <c r="K135" s="12"/>
+      <c r="L135" s="12"/>
+      <c r="M135" s="12"/>
+      <c r="N135" s="12"/>
+      <c r="O135" s="12"/>
+    </row>
+    <row r="136" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C136" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D136" s="3"/>
+      <c r="E136" s="5"/>
+      <c r="F136" s="5"/>
+      <c r="G136" s="5"/>
+      <c r="H136" s="5"/>
+      <c r="I136" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J136" s="3"/>
+      <c r="K136" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L136" s="5"/>
+      <c r="M136" s="5"/>
+      <c r="N136" s="5"/>
+      <c r="O136" s="5"/>
+    </row>
+    <row r="137" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C137" s="3"/>
+      <c r="D137" s="3"/>
+      <c r="E137" s="5"/>
+      <c r="F137" s="5"/>
+      <c r="G137" s="5"/>
+      <c r="H137" s="5"/>
+      <c r="I137" s="3"/>
+      <c r="J137" s="3"/>
+      <c r="K137" s="5"/>
+      <c r="L137" s="5"/>
+      <c r="M137" s="5"/>
+      <c r="N137" s="5"/>
+      <c r="O137" s="5"/>
+    </row>
+    <row r="138" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C138" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D138" s="7"/>
+      <c r="E138" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F138" s="5"/>
+      <c r="G138" s="5"/>
+      <c r="H138" s="5"/>
+      <c r="I138" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J138" s="3"/>
+      <c r="K138" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L138" s="2"/>
+      <c r="M138" s="2"/>
+      <c r="N138" s="2"/>
+      <c r="O138" s="2"/>
+    </row>
+    <row r="139" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C139" s="8"/>
+      <c r="D139" s="9"/>
+      <c r="E139" s="5"/>
+      <c r="F139" s="5"/>
+      <c r="G139" s="5"/>
+      <c r="H139" s="5"/>
+      <c r="I139" s="3"/>
+      <c r="J139" s="3"/>
+      <c r="K139" s="2"/>
+      <c r="L139" s="2"/>
+      <c r="M139" s="2"/>
+      <c r="N139" s="2"/>
+      <c r="O139" s="2"/>
+    </row>
+    <row r="141" spans="3:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="C141" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D141" s="10"/>
+      <c r="E141" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F141" s="3"/>
+      <c r="G141" s="3"/>
+      <c r="H141" s="3"/>
+      <c r="I141" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J141" s="3"/>
+      <c r="K141" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L141" s="3"/>
+      <c r="M141" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N141" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O141" s="3"/>
+    </row>
+    <row r="142" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C142" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D142" s="3"/>
+      <c r="E142" s="4"/>
+      <c r="F142" s="4"/>
+      <c r="G142" s="4"/>
+      <c r="H142" s="4"/>
+      <c r="I142" s="4"/>
+      <c r="J142" s="4"/>
+      <c r="K142" s="4"/>
+      <c r="L142" s="4"/>
+      <c r="M142" s="4"/>
+      <c r="N142" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O142" s="2"/>
+    </row>
+    <row r="143" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C143" s="3"/>
+      <c r="D143" s="3"/>
+      <c r="E143" s="4"/>
+      <c r="F143" s="4"/>
+      <c r="G143" s="4"/>
+      <c r="H143" s="4"/>
+      <c r="I143" s="4"/>
+      <c r="J143" s="4"/>
+      <c r="K143" s="4"/>
+      <c r="L143" s="4"/>
+      <c r="M143" s="4"/>
+      <c r="N143" s="2"/>
+      <c r="O143" s="2"/>
+    </row>
+    <row r="144" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C144" s="3"/>
+      <c r="D144" s="3"/>
+      <c r="E144" s="4"/>
+      <c r="F144" s="4"/>
+      <c r="G144" s="4"/>
+      <c r="H144" s="4"/>
+      <c r="I144" s="4"/>
+      <c r="J144" s="4"/>
+      <c r="K144" s="4"/>
+      <c r="L144" s="4"/>
+      <c r="M144" s="4"/>
+      <c r="N144" s="2"/>
+      <c r="O144" s="2"/>
+    </row>
+    <row r="145" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C145" s="3"/>
+      <c r="D145" s="3"/>
+      <c r="E145" s="4"/>
+      <c r="F145" s="4"/>
+      <c r="G145" s="4"/>
+      <c r="H145" s="4"/>
+      <c r="I145" s="4"/>
+      <c r="J145" s="4"/>
+      <c r="K145" s="4"/>
+      <c r="L145" s="4"/>
+      <c r="M145" s="4"/>
+      <c r="N145" s="2"/>
+      <c r="O145" s="2"/>
+    </row>
+    <row r="146" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C146" s="3"/>
+      <c r="D146" s="3"/>
+      <c r="E146" s="4"/>
+      <c r="F146" s="4"/>
+      <c r="G146" s="4"/>
+      <c r="H146" s="4"/>
+      <c r="I146" s="4"/>
+      <c r="J146" s="4"/>
+      <c r="K146" s="4"/>
+      <c r="L146" s="4"/>
+      <c r="M146" s="4"/>
+      <c r="N146" s="2"/>
+      <c r="O146" s="2"/>
+    </row>
+    <row r="150" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C150" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D150" s="11"/>
+      <c r="E150" s="11"/>
+      <c r="F150" s="11"/>
+      <c r="G150" s="11"/>
+      <c r="H150" s="11"/>
+      <c r="I150" s="11"/>
+      <c r="J150" s="11"/>
+      <c r="K150" s="11"/>
+      <c r="L150" s="11"/>
+      <c r="M150" s="11"/>
+      <c r="N150" s="11"/>
+      <c r="O150" s="11"/>
+    </row>
+    <row r="151" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C151" s="11"/>
+      <c r="D151" s="11"/>
+      <c r="E151" s="11"/>
+      <c r="F151" s="11"/>
+      <c r="G151" s="11"/>
+      <c r="H151" s="11"/>
+      <c r="I151" s="11"/>
+      <c r="J151" s="11"/>
+      <c r="K151" s="11"/>
+      <c r="L151" s="11"/>
+      <c r="M151" s="11"/>
+      <c r="N151" s="11"/>
+      <c r="O151" s="11"/>
+    </row>
+    <row r="153" spans="3:15" ht="21" x14ac:dyDescent="0.4">
+      <c r="C153" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D153" s="12"/>
+      <c r="E153" s="12"/>
+      <c r="F153" s="12"/>
+      <c r="G153" s="12"/>
+      <c r="H153" s="12"/>
+      <c r="I153" s="12"/>
+      <c r="J153" s="12"/>
+      <c r="K153" s="12"/>
+      <c r="L153" s="12"/>
+      <c r="M153" s="12"/>
+      <c r="N153" s="12"/>
+      <c r="O153" s="12"/>
+    </row>
+    <row r="154" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C154" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D154" s="3"/>
+      <c r="E154" s="5"/>
+      <c r="F154" s="5"/>
+      <c r="G154" s="5"/>
+      <c r="H154" s="5"/>
+      <c r="I154" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J154" s="3"/>
+      <c r="K154" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L154" s="5"/>
+      <c r="M154" s="5"/>
+      <c r="N154" s="5"/>
+      <c r="O154" s="5"/>
+    </row>
+    <row r="155" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C155" s="3"/>
+      <c r="D155" s="3"/>
+      <c r="E155" s="5"/>
+      <c r="F155" s="5"/>
+      <c r="G155" s="5"/>
+      <c r="H155" s="5"/>
+      <c r="I155" s="3"/>
+      <c r="J155" s="3"/>
+      <c r="K155" s="5"/>
+      <c r="L155" s="5"/>
+      <c r="M155" s="5"/>
+      <c r="N155" s="5"/>
+      <c r="O155" s="5"/>
+    </row>
+    <row r="156" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C156" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D156" s="7"/>
+      <c r="E156" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F156" s="5"/>
+      <c r="G156" s="5"/>
+      <c r="H156" s="5"/>
+      <c r="I156" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J156" s="3"/>
+      <c r="K156" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L156" s="2"/>
+      <c r="M156" s="2"/>
+      <c r="N156" s="2"/>
+      <c r="O156" s="2"/>
+    </row>
+    <row r="157" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C157" s="8"/>
+      <c r="D157" s="9"/>
+      <c r="E157" s="5"/>
+      <c r="F157" s="5"/>
+      <c r="G157" s="5"/>
+      <c r="H157" s="5"/>
+      <c r="I157" s="3"/>
+      <c r="J157" s="3"/>
+      <c r="K157" s="2"/>
+      <c r="L157" s="2"/>
+      <c r="M157" s="2"/>
+      <c r="N157" s="2"/>
+      <c r="O157" s="2"/>
+    </row>
+    <row r="159" spans="3:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="C159" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D159" s="10"/>
+      <c r="E159" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F159" s="3"/>
+      <c r="G159" s="3"/>
+      <c r="H159" s="3"/>
+      <c r="I159" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J159" s="3"/>
+      <c r="K159" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L159" s="3"/>
+      <c r="M159" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N159" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O159" s="3"/>
+    </row>
+    <row r="160" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C160" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D160" s="3"/>
+      <c r="E160" s="4"/>
+      <c r="F160" s="4"/>
+      <c r="G160" s="4"/>
+      <c r="H160" s="4"/>
+      <c r="I160" s="4"/>
+      <c r="J160" s="4"/>
+      <c r="K160" s="4"/>
+      <c r="L160" s="4"/>
+      <c r="M160" s="4"/>
+      <c r="N160" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O160" s="2"/>
+    </row>
+    <row r="161" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C161" s="3"/>
+      <c r="D161" s="3"/>
+      <c r="E161" s="4"/>
+      <c r="F161" s="4"/>
+      <c r="G161" s="4"/>
+      <c r="H161" s="4"/>
+      <c r="I161" s="4"/>
+      <c r="J161" s="4"/>
+      <c r="K161" s="4"/>
+      <c r="L161" s="4"/>
+      <c r="M161" s="4"/>
+      <c r="N161" s="2"/>
+      <c r="O161" s="2"/>
+    </row>
+    <row r="162" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C162" s="3"/>
+      <c r="D162" s="3"/>
+      <c r="E162" s="4"/>
+      <c r="F162" s="4"/>
+      <c r="G162" s="4"/>
+      <c r="H162" s="4"/>
+      <c r="I162" s="4"/>
+      <c r="J162" s="4"/>
+      <c r="K162" s="4"/>
+      <c r="L162" s="4"/>
+      <c r="M162" s="4"/>
+      <c r="N162" s="2"/>
+      <c r="O162" s="2"/>
+    </row>
+    <row r="163" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C163" s="3"/>
+      <c r="D163" s="3"/>
+      <c r="E163" s="4"/>
+      <c r="F163" s="4"/>
+      <c r="G163" s="4"/>
+      <c r="H163" s="4"/>
+      <c r="I163" s="4"/>
+      <c r="J163" s="4"/>
+      <c r="K163" s="4"/>
+      <c r="L163" s="4"/>
+      <c r="M163" s="4"/>
+      <c r="N163" s="2"/>
+      <c r="O163" s="2"/>
+    </row>
+    <row r="164" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C164" s="3"/>
+      <c r="D164" s="3"/>
+      <c r="E164" s="4"/>
+      <c r="F164" s="4"/>
+      <c r="G164" s="4"/>
+      <c r="H164" s="4"/>
+      <c r="I164" s="4"/>
+      <c r="J164" s="4"/>
+      <c r="K164" s="4"/>
+      <c r="L164" s="4"/>
+      <c r="M164" s="4"/>
+      <c r="N164" s="2"/>
+      <c r="O164" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="190">
+    <mergeCell ref="C160:D164"/>
+    <mergeCell ref="E160:H164"/>
+    <mergeCell ref="I160:J164"/>
+    <mergeCell ref="K160:L164"/>
+    <mergeCell ref="M160:M164"/>
+    <mergeCell ref="N160:O164"/>
+    <mergeCell ref="C156:D157"/>
+    <mergeCell ref="E156:H157"/>
+    <mergeCell ref="I156:J157"/>
+    <mergeCell ref="K156:O157"/>
+    <mergeCell ref="C159:D159"/>
+    <mergeCell ref="E159:H159"/>
+    <mergeCell ref="I159:J159"/>
+    <mergeCell ref="K159:L159"/>
+    <mergeCell ref="N159:O159"/>
+    <mergeCell ref="C150:O151"/>
+    <mergeCell ref="C153:O153"/>
+    <mergeCell ref="C154:D155"/>
+    <mergeCell ref="E154:H155"/>
+    <mergeCell ref="I154:J155"/>
+    <mergeCell ref="K154:O155"/>
+    <mergeCell ref="C142:D146"/>
+    <mergeCell ref="E142:H146"/>
+    <mergeCell ref="I142:J146"/>
+    <mergeCell ref="K142:L146"/>
+    <mergeCell ref="M142:M146"/>
+    <mergeCell ref="N142:O146"/>
+    <mergeCell ref="C138:D139"/>
+    <mergeCell ref="E138:H139"/>
+    <mergeCell ref="I138:J139"/>
+    <mergeCell ref="K138:O139"/>
+    <mergeCell ref="C141:D141"/>
+    <mergeCell ref="E141:H141"/>
+    <mergeCell ref="I141:J141"/>
+    <mergeCell ref="K141:L141"/>
+    <mergeCell ref="N141:O141"/>
+    <mergeCell ref="C132:O133"/>
+    <mergeCell ref="C135:O135"/>
+    <mergeCell ref="C136:D137"/>
+    <mergeCell ref="E136:H137"/>
+    <mergeCell ref="I136:J137"/>
+    <mergeCell ref="K136:O137"/>
+    <mergeCell ref="C124:D128"/>
+    <mergeCell ref="E124:H128"/>
+    <mergeCell ref="I124:J128"/>
+    <mergeCell ref="K124:L128"/>
+    <mergeCell ref="M124:M128"/>
+    <mergeCell ref="N124:O128"/>
+    <mergeCell ref="C120:D121"/>
+    <mergeCell ref="E120:H121"/>
+    <mergeCell ref="I120:J121"/>
+    <mergeCell ref="K120:O121"/>
+    <mergeCell ref="C123:D123"/>
+    <mergeCell ref="E123:H123"/>
+    <mergeCell ref="I123:J123"/>
+    <mergeCell ref="K123:L123"/>
+    <mergeCell ref="N123:O123"/>
+    <mergeCell ref="C114:O115"/>
+    <mergeCell ref="C117:O117"/>
+    <mergeCell ref="C118:D119"/>
+    <mergeCell ref="E118:H119"/>
+    <mergeCell ref="I118:J119"/>
+    <mergeCell ref="K118:O119"/>
+    <mergeCell ref="C106:D110"/>
+    <mergeCell ref="E106:H110"/>
+    <mergeCell ref="I106:J110"/>
+    <mergeCell ref="K106:L110"/>
+    <mergeCell ref="M106:M110"/>
+    <mergeCell ref="N106:O110"/>
+    <mergeCell ref="C102:D103"/>
+    <mergeCell ref="E102:H103"/>
+    <mergeCell ref="I102:J103"/>
+    <mergeCell ref="K102:O103"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="E105:H105"/>
+    <mergeCell ref="I105:J105"/>
+    <mergeCell ref="K105:L105"/>
+    <mergeCell ref="N105:O105"/>
+    <mergeCell ref="C96:O97"/>
+    <mergeCell ref="C99:O99"/>
+    <mergeCell ref="C100:D101"/>
+    <mergeCell ref="E100:H101"/>
+    <mergeCell ref="I100:J101"/>
+    <mergeCell ref="K100:O101"/>
+    <mergeCell ref="C88:D92"/>
+    <mergeCell ref="E88:H92"/>
+    <mergeCell ref="I88:J92"/>
+    <mergeCell ref="K88:L92"/>
+    <mergeCell ref="M88:M92"/>
+    <mergeCell ref="N88:O92"/>
+    <mergeCell ref="C84:D85"/>
+    <mergeCell ref="E84:H85"/>
+    <mergeCell ref="I84:J85"/>
+    <mergeCell ref="K84:O85"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="E87:H87"/>
+    <mergeCell ref="I87:J87"/>
+    <mergeCell ref="K87:L87"/>
+    <mergeCell ref="N87:O87"/>
+    <mergeCell ref="C78:O79"/>
+    <mergeCell ref="C81:O81"/>
+    <mergeCell ref="C82:D83"/>
+    <mergeCell ref="E82:H83"/>
+    <mergeCell ref="I82:J83"/>
+    <mergeCell ref="K82:O83"/>
+    <mergeCell ref="C70:D74"/>
+    <mergeCell ref="E70:H74"/>
+    <mergeCell ref="I70:J74"/>
+    <mergeCell ref="K70:L74"/>
+    <mergeCell ref="M70:M74"/>
+    <mergeCell ref="N70:O74"/>
+    <mergeCell ref="C66:D67"/>
+    <mergeCell ref="E66:H67"/>
+    <mergeCell ref="I66:J67"/>
+    <mergeCell ref="K66:O67"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="E69:H69"/>
+    <mergeCell ref="I69:J69"/>
+    <mergeCell ref="K69:L69"/>
+    <mergeCell ref="N69:O69"/>
+    <mergeCell ref="C60:O61"/>
+    <mergeCell ref="C63:O63"/>
+    <mergeCell ref="C64:D65"/>
+    <mergeCell ref="E64:H65"/>
+    <mergeCell ref="I64:J65"/>
+    <mergeCell ref="K64:O65"/>
+    <mergeCell ref="C52:D56"/>
+    <mergeCell ref="E52:H56"/>
+    <mergeCell ref="I52:J56"/>
+    <mergeCell ref="K52:L56"/>
+    <mergeCell ref="M52:M56"/>
+    <mergeCell ref="N52:O56"/>
+    <mergeCell ref="C48:D49"/>
+    <mergeCell ref="E48:H49"/>
+    <mergeCell ref="I48:J49"/>
+    <mergeCell ref="K48:O49"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="E51:H51"/>
+    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="K51:L51"/>
+    <mergeCell ref="N51:O51"/>
+    <mergeCell ref="C42:O43"/>
+    <mergeCell ref="C45:O45"/>
+    <mergeCell ref="C46:D47"/>
+    <mergeCell ref="E46:H47"/>
+    <mergeCell ref="I46:J47"/>
+    <mergeCell ref="K46:O47"/>
+    <mergeCell ref="C34:D38"/>
+    <mergeCell ref="E34:H38"/>
+    <mergeCell ref="I34:J38"/>
+    <mergeCell ref="K34:L38"/>
+    <mergeCell ref="M34:M38"/>
+    <mergeCell ref="N34:O38"/>
+    <mergeCell ref="C30:D31"/>
+    <mergeCell ref="E30:H31"/>
+    <mergeCell ref="I30:J31"/>
+    <mergeCell ref="K30:O31"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="C24:O25"/>
+    <mergeCell ref="C27:O27"/>
+    <mergeCell ref="C28:D29"/>
+    <mergeCell ref="E28:H29"/>
+    <mergeCell ref="I28:J29"/>
+    <mergeCell ref="K28:O29"/>
+    <mergeCell ref="C16:D20"/>
+    <mergeCell ref="E16:H20"/>
+    <mergeCell ref="I16:J20"/>
+    <mergeCell ref="K16:L20"/>
+    <mergeCell ref="M16:M20"/>
+    <mergeCell ref="N16:O20"/>
+    <mergeCell ref="C12:D13"/>
+    <mergeCell ref="E12:H13"/>
+    <mergeCell ref="I12:J13"/>
+    <mergeCell ref="K12:O13"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="C1:O4"/>
+    <mergeCell ref="C6:O7"/>
+    <mergeCell ref="C9:O9"/>
+    <mergeCell ref="C10:D11"/>
+    <mergeCell ref="E10:H11"/>
+    <mergeCell ref="I10:J11"/>
+    <mergeCell ref="K10:O11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F4FE71-C6FC-40D1-BEB8-75091FEF9EE0}">
+  <dimension ref="C1:O56"/>
+  <sheetViews>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42:O43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="12" max="12" width="18.88671875" customWidth="1"/>
+    <col min="13" max="13" width="27.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+    </row>
+    <row r="2" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+    </row>
+    <row r="3" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+    </row>
+    <row r="4" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+    </row>
     <row r="6" spans="3:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="11" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
@@ -1680,7 +4092,7 @@
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
@@ -1690,7 +4102,7 @@
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
@@ -1718,7 +4130,7 @@
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
@@ -1783,21 +4195,21 @@
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>12</v>
@@ -1866,7 +4278,7 @@
     </row>
     <row r="24" spans="3:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="11" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
@@ -1919,7 +4331,7 @@
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -1929,7 +4341,7 @@
       </c>
       <c r="J28" s="3"/>
       <c r="K28" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
@@ -1957,7 +4369,7 @@
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
@@ -2018,25 +4430,25 @@
     </row>
     <row r="34" spans="3:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C34" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L34" s="4"/>
       <c r="M34" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N34" s="2" t="s">
         <v>12</v>
@@ -2105,7 +4517,7 @@
     </row>
     <row r="42" spans="3:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C42" s="11" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="11"/>
@@ -2158,7 +4570,7 @@
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
@@ -2168,7 +4580,7 @@
       </c>
       <c r="J46" s="3"/>
       <c r="K46" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L46" s="5"/>
       <c r="M46" s="5"/>
@@ -2196,7 +4608,7 @@
       </c>
       <c r="D48" s="7"/>
       <c r="E48" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
@@ -2257,25 +4669,25 @@
     </row>
     <row r="52" spans="3:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C52" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
       <c r="I52" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J52" s="5"/>
       <c r="K52" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="L52" s="4"/>
       <c r="M52" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N52" s="2" t="s">
         <v>12</v>
@@ -2413,12 +4825,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29AC1733-AB24-4039-86F2-A980D2CD8727}">
   <dimension ref="C1:O74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="Q70" sqref="Q70"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60:O61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2429,7 +4841,7 @@
   <sheetData>
     <row r="1" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C1" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
@@ -2491,7 +4903,7 @@
     </row>
     <row r="6" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C6" s="11" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
@@ -2544,7 +4956,7 @@
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -2554,7 +4966,7 @@
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
@@ -2582,7 +4994,7 @@
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -2643,25 +5055,25 @@
     </row>
     <row r="16" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C16" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>12</v>
@@ -2730,7 +5142,7 @@
     </row>
     <row r="24" spans="3:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="11" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
@@ -2783,7 +5195,7 @@
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -2793,7 +5205,7 @@
       </c>
       <c r="J28" s="3"/>
       <c r="K28" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
@@ -2821,7 +5233,7 @@
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
@@ -2886,21 +5298,21 @@
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L34" s="4"/>
       <c r="M34" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N34" s="2" t="s">
         <v>12</v>
@@ -2969,7 +5381,7 @@
     </row>
     <row r="42" spans="3:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C42" s="11" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="11"/>
@@ -3022,7 +5434,7 @@
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
@@ -3032,7 +5444,7 @@
       </c>
       <c r="J46" s="3"/>
       <c r="K46" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L46" s="5"/>
       <c r="M46" s="5"/>
@@ -3060,7 +5472,7 @@
       </c>
       <c r="D48" s="7"/>
       <c r="E48" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
@@ -3121,25 +5533,25 @@
     </row>
     <row r="52" spans="3:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C52" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
       <c r="I52" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J52" s="4"/>
       <c r="K52" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L52" s="4"/>
       <c r="M52" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N52" s="2" t="s">
         <v>12</v>
@@ -3208,7 +5620,7 @@
     </row>
     <row r="60" spans="3:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C60" s="11" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="D60" s="11"/>
       <c r="E60" s="11"/>
@@ -3261,7 +5673,7 @@
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
@@ -3271,7 +5683,7 @@
       </c>
       <c r="J64" s="3"/>
       <c r="K64" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L64" s="5"/>
       <c r="M64" s="5"/>
@@ -3299,7 +5711,7 @@
       </c>
       <c r="D66" s="7"/>
       <c r="E66" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F66" s="5"/>
       <c r="G66" s="5"/>
@@ -3360,25 +5772,25 @@
     </row>
     <row r="70" spans="3:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C70" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D70" s="3"/>
       <c r="E70" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
       <c r="I70" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J70" s="5"/>
       <c r="K70" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="L70" s="4"/>
       <c r="M70" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N70" s="2" t="s">
         <v>12</v>
@@ -3535,4 +5947,348 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DA3CCF6-35D0-48EB-99AF-55CC6B1FD822}">
+  <dimension ref="C1:O20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16:J20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="12" max="12" width="11.44140625" customWidth="1"/>
+    <col min="13" max="13" width="24.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C1" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+    </row>
+    <row r="2" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+    </row>
+    <row r="3" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+    </row>
+    <row r="4" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C6" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+    </row>
+    <row r="9" spans="3:15" ht="21" x14ac:dyDescent="0.4">
+      <c r="C9" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="K10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C13" s="8"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+    </row>
+    <row r="15" spans="3:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="C15" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L15" s="3"/>
+      <c r="M15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C16" s="3">
+        <v>20</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="L16" s="4"/>
+      <c r="M16" s="14">
+        <v>1</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O16" s="2"/>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="22">
+    <mergeCell ref="C16:D20"/>
+    <mergeCell ref="E16:H20"/>
+    <mergeCell ref="I16:J20"/>
+    <mergeCell ref="K16:L20"/>
+    <mergeCell ref="M16:M20"/>
+    <mergeCell ref="N16:O20"/>
+    <mergeCell ref="C12:D13"/>
+    <mergeCell ref="E12:H13"/>
+    <mergeCell ref="I12:J13"/>
+    <mergeCell ref="K12:O13"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="C1:O4"/>
+    <mergeCell ref="C6:O7"/>
+    <mergeCell ref="C9:O9"/>
+    <mergeCell ref="C10:D11"/>
+    <mergeCell ref="E10:H11"/>
+    <mergeCell ref="I10:J11"/>
+    <mergeCell ref="K10:O11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add gameplay sheet to QA documentation
Co-Authored-By: Stoyan Skuliev <106760018+SGSkuliev21@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/Baklava_-_QA_Documentation.xlsx
+++ b/docs/Baklava_-_QA_Documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivelin\Documents\baklava\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4DD221-BAD1-4A8F-9CF9-BA0FFC7BAB48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42ED5331-F5DB-4047-BB48-C99573BC0022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{15209598-3E61-4671-B5D6-5F4A7C929687}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{15209598-3E61-4671-B5D6-5F4A7C929687}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Menu" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="106">
   <si>
     <t>Test Case 1</t>
   </si>
@@ -128,9 +128,6 @@
     <t>№ 10</t>
   </si>
   <si>
-    <t>Check if play button works</t>
-  </si>
-  <si>
     <t>Functionality</t>
   </si>
   <si>
@@ -140,18 +137,12 @@
     <t>Menu button check</t>
   </si>
   <si>
-    <t xml:space="preserve">When the user clicks the button the scene changes and realises him in the game </t>
-  </si>
-  <si>
     <t>The user clicks on quit button and the game closes</t>
   </si>
   <si>
     <t xml:space="preserve">When the user clicks the button the scene changes and the game closes </t>
   </si>
   <si>
-    <t>The user clicks on play button and the game starts</t>
-  </si>
-  <si>
     <t>Check if esc key closes game</t>
   </si>
   <si>
@@ -264,6 +255,108 @@
   </si>
   <si>
     <t>20 | 100.0%</t>
+  </si>
+  <si>
+    <t>Check if camera moves</t>
+  </si>
+  <si>
+    <t>Camera check</t>
+  </si>
+  <si>
+    <t>When you start the game, left click and move your mouse the camera moves</t>
+  </si>
+  <si>
+    <t>When the user starts the game, left clicks and moves his mouse the camera moves</t>
+  </si>
+  <si>
+    <t>Check if upgrade button works</t>
+  </si>
+  <si>
+    <t>When you enter the game on the left there is a upgrade button. If you click it, the button expands</t>
+  </si>
+  <si>
+    <t>Upgrade button check</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When the user enters the game, clicks the upgrades button the button expands </t>
+  </si>
+  <si>
+    <t>When the user enters the game, clicks the upgrades button the button expands</t>
+  </si>
+  <si>
+    <t>Input check</t>
+  </si>
+  <si>
+    <t>When the game starts and you click any number it displays on the top right of the screen</t>
+  </si>
+  <si>
+    <t>When the user starts the game and clicks any number it displays on the top right of the screen</t>
+  </si>
+  <si>
+    <t>Tower shoot check</t>
+  </si>
+  <si>
+    <t>When the game starts and you guess the first math problem the tower shoots the enemy</t>
+  </si>
+  <si>
+    <t>When the user starts the game and guesses the first math problem the tower shoots the enemy</t>
+  </si>
+  <si>
+    <t>Enemy damage check</t>
+  </si>
+  <si>
+    <t>When you enter the game and the enemy hits the tower it does damage on the tower</t>
+  </si>
+  <si>
+    <t>When the user enters the game and the enemy hits the tower it does damage on the tower</t>
+  </si>
+  <si>
+    <t>Enemy movement check</t>
+  </si>
+  <si>
+    <t>When you start the game the enemies start to move towards the tower</t>
+  </si>
+  <si>
+    <t>When the user starts the game the enemies start to move towards the tower</t>
+  </si>
+  <si>
+    <t>The user clicks on the play button and the game starts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When the user clicks the button, the scene changes and releases him into the game </t>
+  </si>
+  <si>
+    <t>Check play button</t>
+  </si>
+  <si>
+    <t>Damage up button check</t>
+  </si>
+  <si>
+    <t>Damage up dutton check</t>
+  </si>
+  <si>
+    <t>When you click the damage up button it increases the tower damage</t>
+  </si>
+  <si>
+    <t>When the user clicks the damage up button it increases the tower damage</t>
+  </si>
+  <si>
+    <t>Clicking the "Regen Up" button it increases the tower's health regeneration rate</t>
+  </si>
+  <si>
+    <t>When the user clicks the "Regen up" button it increases the tower's health regeneration rate</t>
+  </si>
+  <si>
+    <t>Multikill up button check</t>
+  </si>
+  <si>
+    <t>Regen up button check</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clicking the "Multikill up" button it increases the enemies killed with one equation  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">When the user clicks the "Multikill up" button it increases the enemies killed with one equation  </t>
   </si>
 </sst>
 </file>
@@ -763,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A3805D7-8844-4E6B-BC59-814E106A8F59}">
   <dimension ref="C1:O56"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="J78" sqref="J78"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -892,7 +985,7 @@
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="5" t="s">
-        <v>29</v>
+        <v>95</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
@@ -930,7 +1023,7 @@
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
@@ -995,21 +1088,21 @@
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="4" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="4" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="4" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>12</v>
@@ -1131,7 +1224,7 @@
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -1169,7 +1262,7 @@
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
@@ -1234,21 +1327,21 @@
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L34" s="4"/>
       <c r="M34" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N34" s="2" t="s">
         <v>12</v>
@@ -1370,7 +1463,7 @@
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
@@ -1408,7 +1501,7 @@
       </c>
       <c r="D48" s="7"/>
       <c r="E48" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
@@ -1473,21 +1566,21 @@
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
       <c r="I52" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="J52" s="5"/>
       <c r="K52" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L52" s="4"/>
       <c r="M52" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="N52" s="2" t="s">
         <v>12</v>
@@ -1630,8 +1723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E38D76E-95FE-4D0A-B5FB-E607E1A67E56}">
   <dimension ref="C1:O164"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C150" sqref="C150:O151"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="M76" sqref="M76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1643,7 +1736,7 @@
   <sheetData>
     <row r="1" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C1" s="13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
@@ -1705,7 +1798,7 @@
     </row>
     <row r="6" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C6" s="11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
@@ -1757,7 +1850,9 @@
         <v>2</v>
       </c>
       <c r="D10" s="3"/>
-      <c r="E10" s="5"/>
+      <c r="E10" s="5" t="s">
+        <v>72</v>
+      </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -1794,7 +1889,7 @@
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
@@ -1858,15 +1953,23 @@
         <v>11</v>
       </c>
       <c r="D16" s="3"/>
-      <c r="E16" s="4"/>
+      <c r="E16" s="4" t="s">
+        <v>74</v>
+      </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
+      <c r="I16" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
+      <c r="K16" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
+      <c r="M16" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="N16" s="2" t="s">
         <v>12</v>
       </c>
@@ -1934,7 +2037,7 @@
     </row>
     <row r="24" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C24" s="11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
@@ -1986,7 +2089,9 @@
         <v>2</v>
       </c>
       <c r="D28" s="3"/>
-      <c r="E28" s="5"/>
+      <c r="E28" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
@@ -2023,7 +2128,7 @@
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
@@ -2087,15 +2192,23 @@
         <v>11</v>
       </c>
       <c r="D34" s="3"/>
-      <c r="E34" s="4"/>
+      <c r="E34" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
+      <c r="I34" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
+      <c r="K34" s="4" t="s">
+        <v>79</v>
+      </c>
       <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
+      <c r="M34" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="N34" s="2" t="s">
         <v>12</v>
       </c>
@@ -2215,7 +2328,9 @@
         <v>2</v>
       </c>
       <c r="D46" s="3"/>
-      <c r="E46" s="5"/>
+      <c r="E46" s="5" t="s">
+        <v>96</v>
+      </c>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
@@ -2252,7 +2367,7 @@
       </c>
       <c r="D48" s="7"/>
       <c r="E48" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
@@ -2316,15 +2431,23 @@
         <v>11</v>
       </c>
       <c r="D52" s="3"/>
-      <c r="E52" s="4"/>
+      <c r="E52" s="4" t="s">
+        <v>98</v>
+      </c>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
-      <c r="I52" s="4"/>
+      <c r="I52" s="4" t="s">
+        <v>97</v>
+      </c>
       <c r="J52" s="4"/>
-      <c r="K52" s="4"/>
+      <c r="K52" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="L52" s="4"/>
-      <c r="M52" s="4"/>
+      <c r="M52" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="N52" s="2" t="s">
         <v>12</v>
       </c>
@@ -2444,7 +2567,9 @@
         <v>2</v>
       </c>
       <c r="D64" s="3"/>
-      <c r="E64" s="5"/>
+      <c r="E64" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
       <c r="H64" s="5"/>
@@ -2481,7 +2606,7 @@
       </c>
       <c r="D66" s="7"/>
       <c r="E66" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F66" s="5"/>
       <c r="G66" s="5"/>
@@ -2545,15 +2670,23 @@
         <v>11</v>
       </c>
       <c r="D70" s="3"/>
-      <c r="E70" s="4"/>
+      <c r="E70" s="4" t="s">
+        <v>104</v>
+      </c>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
-      <c r="I70" s="4"/>
+      <c r="I70" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="J70" s="4"/>
-      <c r="K70" s="4"/>
+      <c r="K70" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="L70" s="4"/>
-      <c r="M70" s="4"/>
+      <c r="M70" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="N70" s="2" t="s">
         <v>12</v>
       </c>
@@ -2673,7 +2806,9 @@
         <v>2</v>
       </c>
       <c r="D82" s="3"/>
-      <c r="E82" s="5"/>
+      <c r="E82" s="5" t="s">
+        <v>103</v>
+      </c>
       <c r="F82" s="5"/>
       <c r="G82" s="5"/>
       <c r="H82" s="5"/>
@@ -2710,7 +2845,7 @@
       </c>
       <c r="D84" s="7"/>
       <c r="E84" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F84" s="5"/>
       <c r="G84" s="5"/>
@@ -2774,15 +2909,23 @@
         <v>11</v>
       </c>
       <c r="D88" s="3"/>
-      <c r="E88" s="4"/>
+      <c r="E88" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="F88" s="4"/>
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
-      <c r="I88" s="4"/>
+      <c r="I88" s="4" t="s">
+        <v>103</v>
+      </c>
       <c r="J88" s="4"/>
-      <c r="K88" s="4"/>
+      <c r="K88" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="L88" s="4"/>
-      <c r="M88" s="4"/>
+      <c r="M88" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="N88" s="2" t="s">
         <v>12</v>
       </c>
@@ -2850,7 +2993,7 @@
     </row>
     <row r="96" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C96" s="11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D96" s="11"/>
       <c r="E96" s="11"/>
@@ -2902,7 +3045,9 @@
         <v>2</v>
       </c>
       <c r="D100" s="3"/>
-      <c r="E100" s="5"/>
+      <c r="E100" s="5" t="s">
+        <v>81</v>
+      </c>
       <c r="F100" s="5"/>
       <c r="G100" s="5"/>
       <c r="H100" s="5"/>
@@ -2939,7 +3084,7 @@
       </c>
       <c r="D102" s="7"/>
       <c r="E102" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F102" s="5"/>
       <c r="G102" s="5"/>
@@ -3003,15 +3148,23 @@
         <v>11</v>
       </c>
       <c r="D106" s="3"/>
-      <c r="E106" s="4"/>
+      <c r="E106" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="F106" s="4"/>
       <c r="G106" s="4"/>
       <c r="H106" s="4"/>
-      <c r="I106" s="4"/>
+      <c r="I106" s="4" t="s">
+        <v>81</v>
+      </c>
       <c r="J106" s="4"/>
-      <c r="K106" s="4"/>
+      <c r="K106" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="L106" s="4"/>
-      <c r="M106" s="4"/>
+      <c r="M106" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="N106" s="2" t="s">
         <v>12</v>
       </c>
@@ -3131,7 +3284,9 @@
         <v>2</v>
       </c>
       <c r="D118" s="3"/>
-      <c r="E118" s="5"/>
+      <c r="E118" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="F118" s="5"/>
       <c r="G118" s="5"/>
       <c r="H118" s="5"/>
@@ -3168,7 +3323,7 @@
       </c>
       <c r="D120" s="7"/>
       <c r="E120" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F120" s="5"/>
       <c r="G120" s="5"/>
@@ -3232,15 +3387,23 @@
         <v>11</v>
       </c>
       <c r="D124" s="3"/>
-      <c r="E124" s="4"/>
+      <c r="E124" s="4" t="s">
+        <v>85</v>
+      </c>
       <c r="F124" s="4"/>
       <c r="G124" s="4"/>
       <c r="H124" s="4"/>
-      <c r="I124" s="4"/>
+      <c r="I124" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="J124" s="4"/>
-      <c r="K124" s="4"/>
+      <c r="K124" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="L124" s="4"/>
-      <c r="M124" s="4"/>
+      <c r="M124" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="N124" s="2" t="s">
         <v>12</v>
       </c>
@@ -3360,7 +3523,9 @@
         <v>2</v>
       </c>
       <c r="D136" s="3"/>
-      <c r="E136" s="5"/>
+      <c r="E136" s="5" t="s">
+        <v>87</v>
+      </c>
       <c r="F136" s="5"/>
       <c r="G136" s="5"/>
       <c r="H136" s="5"/>
@@ -3397,7 +3562,7 @@
       </c>
       <c r="D138" s="7"/>
       <c r="E138" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F138" s="5"/>
       <c r="G138" s="5"/>
@@ -3461,15 +3626,23 @@
         <v>11</v>
       </c>
       <c r="D142" s="3"/>
-      <c r="E142" s="4"/>
+      <c r="E142" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="F142" s="4"/>
       <c r="G142" s="4"/>
       <c r="H142" s="4"/>
-      <c r="I142" s="4"/>
+      <c r="I142" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="J142" s="4"/>
-      <c r="K142" s="4"/>
+      <c r="K142" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="L142" s="4"/>
-      <c r="M142" s="4"/>
+      <c r="M142" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="N142" s="2" t="s">
         <v>12</v>
       </c>
@@ -3589,7 +3762,9 @@
         <v>2</v>
       </c>
       <c r="D154" s="3"/>
-      <c r="E154" s="5"/>
+      <c r="E154" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="F154" s="5"/>
       <c r="G154" s="5"/>
       <c r="H154" s="5"/>
@@ -3626,7 +3801,7 @@
       </c>
       <c r="D156" s="7"/>
       <c r="E156" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F156" s="5"/>
       <c r="G156" s="5"/>
@@ -3690,15 +3865,23 @@
         <v>11</v>
       </c>
       <c r="D160" s="3"/>
-      <c r="E160" s="4"/>
+      <c r="E160" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F160" s="4"/>
       <c r="G160" s="4"/>
       <c r="H160" s="4"/>
-      <c r="I160" s="4"/>
+      <c r="I160" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="J160" s="4"/>
-      <c r="K160" s="4"/>
+      <c r="K160" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="L160" s="4"/>
-      <c r="M160" s="4"/>
+      <c r="M160" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="N160" s="2" t="s">
         <v>12</v>
       </c>
@@ -3965,7 +4148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F4FE71-C6FC-40D1-BEB8-75091FEF9EE0}">
   <dimension ref="C1:O56"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C42" sqref="C42:O43"/>
     </sheetView>
   </sheetViews>
@@ -4092,7 +4275,7 @@
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
@@ -4130,7 +4313,7 @@
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
@@ -4195,21 +4378,21 @@
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>12</v>
@@ -4331,7 +4514,7 @@
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -4369,7 +4552,7 @@
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
@@ -4434,21 +4617,21 @@
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L34" s="4"/>
       <c r="M34" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N34" s="2" t="s">
         <v>12</v>
@@ -4517,7 +4700,7 @@
     </row>
     <row r="42" spans="3:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C42" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="11"/>
@@ -4570,7 +4753,7 @@
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
@@ -4608,7 +4791,7 @@
       </c>
       <c r="D48" s="7"/>
       <c r="E48" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
@@ -4673,21 +4856,21 @@
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
       <c r="I52" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="J52" s="5"/>
       <c r="K52" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L52" s="4"/>
       <c r="M52" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="N52" s="2" t="s">
         <v>12</v>
@@ -4841,7 +5024,7 @@
   <sheetData>
     <row r="1" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C1" s="13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
@@ -4903,7 +5086,7 @@
     </row>
     <row r="6" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C6" s="11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
@@ -4956,7 +5139,7 @@
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -4994,7 +5177,7 @@
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -5059,21 +5242,21 @@
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>12</v>
@@ -5142,7 +5325,7 @@
     </row>
     <row r="24" spans="3:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
@@ -5195,7 +5378,7 @@
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -5233,7 +5416,7 @@
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
@@ -5298,21 +5481,21 @@
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L34" s="4"/>
       <c r="M34" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="N34" s="2" t="s">
         <v>12</v>
@@ -5381,7 +5564,7 @@
     </row>
     <row r="42" spans="3:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C42" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="11"/>
@@ -5434,7 +5617,7 @@
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
@@ -5472,7 +5655,7 @@
       </c>
       <c r="D48" s="7"/>
       <c r="E48" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
@@ -5537,21 +5720,21 @@
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
       <c r="I52" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J52" s="4"/>
       <c r="K52" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L52" s="4"/>
       <c r="M52" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N52" s="2" t="s">
         <v>12</v>
@@ -5620,7 +5803,7 @@
     </row>
     <row r="60" spans="3:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C60" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D60" s="11"/>
       <c r="E60" s="11"/>
@@ -5673,7 +5856,7 @@
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
@@ -5711,7 +5894,7 @@
       </c>
       <c r="D66" s="7"/>
       <c r="E66" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F66" s="5"/>
       <c r="G66" s="5"/>
@@ -5776,21 +5959,21 @@
       </c>
       <c r="D70" s="3"/>
       <c r="E70" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
       <c r="I70" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="J70" s="5"/>
       <c r="K70" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L70" s="4"/>
       <c r="M70" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="N70" s="2" t="s">
         <v>12</v>
@@ -5953,7 +6136,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DA3CCF6-35D0-48EB-99AF-55CC6B1FD822}">
   <dimension ref="C1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I16" sqref="I16:J20"/>
     </sheetView>
   </sheetViews>
@@ -5965,7 +6148,7 @@
   <sheetData>
     <row r="1" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C1" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
@@ -6027,7 +6210,7 @@
     </row>
     <row r="6" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C6" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
@@ -6080,7 +6263,7 @@
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
@@ -6114,11 +6297,11 @@
     </row>
     <row r="12" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C12" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
@@ -6152,25 +6335,25 @@
     </row>
     <row r="15" spans="3:15" ht="18" x14ac:dyDescent="0.35">
       <c r="C15" s="10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="L15" s="3"/>
       <c r="M15" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="N15" s="3" t="s">
         <v>5</v>
@@ -6183,17 +6366,17 @@
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="14">

</xml_diff>